<commit_message>
-Correcting some documentation issues
</commit_message>
<xml_diff>
--- a/H0FR72/Released/BOM/H0FR72.xlsx
+++ b/H0FR72/Released/BOM/H0FR72.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H0FR7x-Hardware\H0FR72\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A66AC54-23C2-4992-99D4-F65F0E3A78ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754CBF05-728B-4AFC-8256-B845455C3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="255" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,7 +787,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2174599</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>16192</xdr:rowOff>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1650,7 @@
         <v>35</v>
       </c>
       <c r="F29" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
-Add additional 10u capacitor to gate driver IC supply
</commit_message>
<xml_diff>
--- a/H0FR72/Released/BOM/H0FR72.xlsx
+++ b/H0FR72/Released/BOM/H0FR72.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H0FR7x-Hardware\H0FR72\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754CBF05-728B-4AFC-8256-B845455C3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7B794A-4AA1-4056-B292-6F1D2C61A9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="255" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H0FR72" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="137">
   <si>
     <t>Description</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>https://octopart.com/vlmo1300-gs08-vishay-21709200?r=sp</t>
+  </si>
+  <si>
+    <t>GRM21BR6YA106ME43K</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>Cap 10UF 35VDC X5R 20% SMD 0805 Embossed Tape</t>
+  </si>
+  <si>
+    <t>https://octopart.com/grm21br6ya106me43k-murata-57368791?r=sp</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G33"/>
+  <dimension ref="A2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1515,39 +1527,39 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E24" s="15" t="s">
         <v>131</v>
-      </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="F24" s="16">
         <v>1</v>
@@ -1555,19 +1567,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F25" s="16">
         <v>1</v>
@@ -1575,19 +1587,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
       <c r="F26" s="16">
         <v>1</v>
@@ -1595,79 +1607,79 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E28" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="F28" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C29" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="F29" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="F30" s="16">
         <v>1</v>
@@ -1675,19 +1687,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="F31" s="16">
         <v>1</v>
@@ -1695,19 +1707,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F32" s="16">
         <v>1</v>
@@ -1715,21 +1727,41 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B34" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E34" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F34" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1740,16 +1772,16 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E25" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E25" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E31" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E26" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E31" r:id="rId8" xr:uid="{F3DD4184-677E-4B08-BF00-1BD27946DA11}"/>
-    <hyperlink ref="E32" r:id="rId9" xr:uid="{A230C74B-FBBB-4165-B19A-19D18F7101BF}"/>
-    <hyperlink ref="E28" r:id="rId10" xr:uid="{235F6EA1-6A98-4FD3-AA97-79EB21C917DB}"/>
+    <hyperlink ref="E32" r:id="rId8" xr:uid="{F3DD4184-677E-4B08-BF00-1BD27946DA11}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{A230C74B-FBBB-4165-B19A-19D18F7101BF}"/>
+    <hyperlink ref="E29" r:id="rId10" xr:uid="{235F6EA1-6A98-4FD3-AA97-79EB21C917DB}"/>
     <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>